<commit_message>
Updated FIN_grids model - 2025-08-26 14:54
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_FIN_grids/Sets-vervestacks.xlsx
@@ -5,16 +5,17 @@
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45088BA-E355-4D59-B6D8-AA94E14D9181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4E33E2-0C74-4C8F-811C-4B569C58E33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
-    <sheet name="VEDA_Sets-Proc" sheetId="1" r:id="rId2"/>
+    <sheet name="geo_sets" sheetId="3" r:id="rId2"/>
+    <sheet name="VEDA_Sets-Proc" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="305">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -328,13 +329,637 @@
   </si>
   <si>
     <t>Transformers Dn</t>
+  </si>
+  <si>
+    <t>~tfm_psets</t>
+  </si>
+  <si>
+    <t>setname</t>
+  </si>
+  <si>
+    <t>pset_co</t>
+  </si>
+  <si>
+    <t>p_FI1</t>
+  </si>
+  <si>
+    <t>e_FI1*</t>
+  </si>
+  <si>
+    <t>p_FI10</t>
+  </si>
+  <si>
+    <t>e_FI10*</t>
+  </si>
+  <si>
+    <t>p_FI11</t>
+  </si>
+  <si>
+    <t>e_FI11*</t>
+  </si>
+  <si>
+    <t>p_FI12</t>
+  </si>
+  <si>
+    <t>e_FI12*</t>
+  </si>
+  <si>
+    <t>p_FI13</t>
+  </si>
+  <si>
+    <t>e_FI13*</t>
+  </si>
+  <si>
+    <t>p_FI14</t>
+  </si>
+  <si>
+    <t>e_FI14*</t>
+  </si>
+  <si>
+    <t>p_FI15</t>
+  </si>
+  <si>
+    <t>e_FI15*</t>
+  </si>
+  <si>
+    <t>p_FI16</t>
+  </si>
+  <si>
+    <t>e_FI16*</t>
+  </si>
+  <si>
+    <t>p_FI17</t>
+  </si>
+  <si>
+    <t>e_FI17*</t>
+  </si>
+  <si>
+    <t>p_FI18</t>
+  </si>
+  <si>
+    <t>e_FI18*</t>
+  </si>
+  <si>
+    <t>p_FI19</t>
+  </si>
+  <si>
+    <t>e_FI19*</t>
+  </si>
+  <si>
+    <t>p_FI2</t>
+  </si>
+  <si>
+    <t>e_FI2*</t>
+  </si>
+  <si>
+    <t>p_FI20</t>
+  </si>
+  <si>
+    <t>e_FI20*</t>
+  </si>
+  <si>
+    <t>p_FI21</t>
+  </si>
+  <si>
+    <t>e_FI21*</t>
+  </si>
+  <si>
+    <t>p_FI22</t>
+  </si>
+  <si>
+    <t>e_FI22*</t>
+  </si>
+  <si>
+    <t>p_FI25</t>
+  </si>
+  <si>
+    <t>e_FI25*</t>
+  </si>
+  <si>
+    <t>p_FI26</t>
+  </si>
+  <si>
+    <t>e_FI26*</t>
+  </si>
+  <si>
+    <t>p_FI27</t>
+  </si>
+  <si>
+    <t>e_FI27*</t>
+  </si>
+  <si>
+    <t>p_FI28</t>
+  </si>
+  <si>
+    <t>e_FI28*</t>
+  </si>
+  <si>
+    <t>p_FI29</t>
+  </si>
+  <si>
+    <t>e_FI29*</t>
+  </si>
+  <si>
+    <t>p_FI3</t>
+  </si>
+  <si>
+    <t>e_FI3*</t>
+  </si>
+  <si>
+    <t>p_FI30</t>
+  </si>
+  <si>
+    <t>e_FI30*</t>
+  </si>
+  <si>
+    <t>p_FI31</t>
+  </si>
+  <si>
+    <t>e_FI31*</t>
+  </si>
+  <si>
+    <t>p_FI32</t>
+  </si>
+  <si>
+    <t>e_FI32*</t>
+  </si>
+  <si>
+    <t>p_FI33</t>
+  </si>
+  <si>
+    <t>e_FI33*</t>
+  </si>
+  <si>
+    <t>p_FI34</t>
+  </si>
+  <si>
+    <t>e_FI34*</t>
+  </si>
+  <si>
+    <t>p_FI35</t>
+  </si>
+  <si>
+    <t>e_FI35*</t>
+  </si>
+  <si>
+    <t>p_FI36</t>
+  </si>
+  <si>
+    <t>e_FI36*</t>
+  </si>
+  <si>
+    <t>p_FI37</t>
+  </si>
+  <si>
+    <t>e_FI37*</t>
+  </si>
+  <si>
+    <t>p_FI38</t>
+  </si>
+  <si>
+    <t>e_FI38*</t>
+  </si>
+  <si>
+    <t>p_FI4</t>
+  </si>
+  <si>
+    <t>e_FI4*</t>
+  </si>
+  <si>
+    <t>p_FI5</t>
+  </si>
+  <si>
+    <t>e_FI5*</t>
+  </si>
+  <si>
+    <t>p_FI6</t>
+  </si>
+  <si>
+    <t>e_FI6*</t>
+  </si>
+  <si>
+    <t>p_FI7</t>
+  </si>
+  <si>
+    <t>e_FI7*</t>
+  </si>
+  <si>
+    <t>p_FI8</t>
+  </si>
+  <si>
+    <t>e_FI8*</t>
+  </si>
+  <si>
+    <t>p_FI9</t>
+  </si>
+  <si>
+    <t>e_FI9*</t>
+  </si>
+  <si>
+    <t>p_r15436115</t>
+  </si>
+  <si>
+    <t>e_r15436115*</t>
+  </si>
+  <si>
+    <t>p_w1107461441</t>
+  </si>
+  <si>
+    <t>e_w1107461441*</t>
+  </si>
+  <si>
+    <t>p_w1155254820</t>
+  </si>
+  <si>
+    <t>e_w1155254820*</t>
+  </si>
+  <si>
+    <t>p_w1159141282</t>
+  </si>
+  <si>
+    <t>e_w1159141282*</t>
+  </si>
+  <si>
+    <t>p_w123462491</t>
+  </si>
+  <si>
+    <t>e_w123462491*</t>
+  </si>
+  <si>
+    <t>p_w1262323677</t>
+  </si>
+  <si>
+    <t>e_w1262323677*</t>
+  </si>
+  <si>
+    <t>p_w1275744419</t>
+  </si>
+  <si>
+    <t>e_w1275744419*</t>
+  </si>
+  <si>
+    <t>p_w128463750</t>
+  </si>
+  <si>
+    <t>e_w128463750*</t>
+  </si>
+  <si>
+    <t>p_w1286130176</t>
+  </si>
+  <si>
+    <t>e_w1286130176*</t>
+  </si>
+  <si>
+    <t>p_w1306874220</t>
+  </si>
+  <si>
+    <t>e_w1306874220*</t>
+  </si>
+  <si>
+    <t>p_w1321685855</t>
+  </si>
+  <si>
+    <t>e_w1321685855*</t>
+  </si>
+  <si>
+    <t>p_w136068907</t>
+  </si>
+  <si>
+    <t>e_w136068907*</t>
+  </si>
+  <si>
+    <t>p_w144383819</t>
+  </si>
+  <si>
+    <t>e_w144383819*</t>
+  </si>
+  <si>
+    <t>p_w144832705</t>
+  </si>
+  <si>
+    <t>e_w144832705*</t>
+  </si>
+  <si>
+    <t>p_w149965733</t>
+  </si>
+  <si>
+    <t>e_w149965733*</t>
+  </si>
+  <si>
+    <t>p_w149965738</t>
+  </si>
+  <si>
+    <t>e_w149965738*</t>
+  </si>
+  <si>
+    <t>p_w149965739</t>
+  </si>
+  <si>
+    <t>e_w149965739*</t>
+  </si>
+  <si>
+    <t>p_w150209972</t>
+  </si>
+  <si>
+    <t>e_w150209972*</t>
+  </si>
+  <si>
+    <t>p_w150282502</t>
+  </si>
+  <si>
+    <t>e_w150282502*</t>
+  </si>
+  <si>
+    <t>p_w151818544</t>
+  </si>
+  <si>
+    <t>e_w151818544*</t>
+  </si>
+  <si>
+    <t>p_w159532385</t>
+  </si>
+  <si>
+    <t>e_w159532385*</t>
+  </si>
+  <si>
+    <t>p_w167705754</t>
+  </si>
+  <si>
+    <t>e_w167705754*</t>
+  </si>
+  <si>
+    <t>p_w169899622</t>
+  </si>
+  <si>
+    <t>e_w169899622*</t>
+  </si>
+  <si>
+    <t>p_w173431802</t>
+  </si>
+  <si>
+    <t>e_w173431802*</t>
+  </si>
+  <si>
+    <t>p_w208979069</t>
+  </si>
+  <si>
+    <t>e_w208979069*</t>
+  </si>
+  <si>
+    <t>p_w217032425</t>
+  </si>
+  <si>
+    <t>e_w217032425*</t>
+  </si>
+  <si>
+    <t>p_w238856422</t>
+  </si>
+  <si>
+    <t>e_w238856422*</t>
+  </si>
+  <si>
+    <t>p_w239242345</t>
+  </si>
+  <si>
+    <t>e_w239242345*</t>
+  </si>
+  <si>
+    <t>p_w26619335</t>
+  </si>
+  <si>
+    <t>e_w26619335*</t>
+  </si>
+  <si>
+    <t>p_w27674611</t>
+  </si>
+  <si>
+    <t>e_w27674611*</t>
+  </si>
+  <si>
+    <t>p_w286955409</t>
+  </si>
+  <si>
+    <t>e_w286955409*</t>
+  </si>
+  <si>
+    <t>p_w28820749</t>
+  </si>
+  <si>
+    <t>e_w28820749*</t>
+  </si>
+  <si>
+    <t>p_w314853393</t>
+  </si>
+  <si>
+    <t>e_w314853393*</t>
+  </si>
+  <si>
+    <t>p_w34623113</t>
+  </si>
+  <si>
+    <t>e_w34623113*</t>
+  </si>
+  <si>
+    <t>p_w348003562</t>
+  </si>
+  <si>
+    <t>e_w348003562*</t>
+  </si>
+  <si>
+    <t>p_w348358044</t>
+  </si>
+  <si>
+    <t>e_w348358044*</t>
+  </si>
+  <si>
+    <t>p_w351960012</t>
+  </si>
+  <si>
+    <t>e_w351960012*</t>
+  </si>
+  <si>
+    <t>p_w35281467</t>
+  </si>
+  <si>
+    <t>e_w35281467*</t>
+  </si>
+  <si>
+    <t>p_w379937972</t>
+  </si>
+  <si>
+    <t>e_w379937972*</t>
+  </si>
+  <si>
+    <t>p_w388655178</t>
+  </si>
+  <si>
+    <t>e_w388655178*</t>
+  </si>
+  <si>
+    <t>p_w388832477</t>
+  </si>
+  <si>
+    <t>e_w388832477*</t>
+  </si>
+  <si>
+    <t>p_w391140226</t>
+  </si>
+  <si>
+    <t>e_w391140226*</t>
+  </si>
+  <si>
+    <t>p_w391142034</t>
+  </si>
+  <si>
+    <t>e_w391142034*</t>
+  </si>
+  <si>
+    <t>p_w391142388</t>
+  </si>
+  <si>
+    <t>e_w391142388*</t>
+  </si>
+  <si>
+    <t>p_w391145068</t>
+  </si>
+  <si>
+    <t>e_w391145068*</t>
+  </si>
+  <si>
+    <t>p_w43143343</t>
+  </si>
+  <si>
+    <t>e_w43143343*</t>
+  </si>
+  <si>
+    <t>p_w47317827</t>
+  </si>
+  <si>
+    <t>e_w47317827*</t>
+  </si>
+  <si>
+    <t>p_w498816162</t>
+  </si>
+  <si>
+    <t>e_w498816162*</t>
+  </si>
+  <si>
+    <t>p_w53047196</t>
+  </si>
+  <si>
+    <t>e_w53047196*</t>
+  </si>
+  <si>
+    <t>p_w544156119</t>
+  </si>
+  <si>
+    <t>e_w544156119*</t>
+  </si>
+  <si>
+    <t>p_w551596913</t>
+  </si>
+  <si>
+    <t>e_w551596913*</t>
+  </si>
+  <si>
+    <t>p_w55275882</t>
+  </si>
+  <si>
+    <t>e_w55275882*</t>
+  </si>
+  <si>
+    <t>p_w55609623</t>
+  </si>
+  <si>
+    <t>e_w55609623*</t>
+  </si>
+  <si>
+    <t>p_w590767557</t>
+  </si>
+  <si>
+    <t>e_w590767557*</t>
+  </si>
+  <si>
+    <t>p_w620351437</t>
+  </si>
+  <si>
+    <t>e_w620351437*</t>
+  </si>
+  <si>
+    <t>p_w671568771</t>
+  </si>
+  <si>
+    <t>e_w671568771*</t>
+  </si>
+  <si>
+    <t>p_w857250602</t>
+  </si>
+  <si>
+    <t>e_w857250602*</t>
+  </si>
+  <si>
+    <t>p_w881741424</t>
+  </si>
+  <si>
+    <t>e_w881741424*</t>
+  </si>
+  <si>
+    <t>p_w95392702</t>
+  </si>
+  <si>
+    <t>e_w95392702*</t>
+  </si>
+  <si>
+    <t>p_w96660466</t>
+  </si>
+  <si>
+    <t>e_w96660466*</t>
+  </si>
+  <si>
+    <t>p_w98561229</t>
+  </si>
+  <si>
+    <t>e_w98561229*</t>
+  </si>
+  <si>
+    <t>p_w98589905</t>
+  </si>
+  <si>
+    <t>e_w98589905*</t>
+  </si>
+  <si>
+    <t>p_w98609844</t>
+  </si>
+  <si>
+    <t>e_w98609844*</t>
+  </si>
+  <si>
+    <t>p_w98613134</t>
+  </si>
+  <si>
+    <t>e_w98613134*</t>
+  </si>
+  <si>
+    <t>p_w98735006</t>
+  </si>
+  <si>
+    <t>e_w98735006*</t>
+  </si>
+  <si>
+    <t>rez_FIN_0</t>
+  </si>
+  <si>
+    <t>elc*FIN_0000</t>
+  </si>
+  <si>
+    <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by vision · Guided by intuition · Fueled by passion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,16 +983,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FF969696"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF19375F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F9FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -393,17 +1063,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -421,6 +1128,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E2985C0-67F7-1572-8736-4A1C56069935}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245100" y="12700"/>
+          <a:ext cx="990600" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,10 +1932,872 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8FACE2-CC4B-4946-A187-073C83DEBD62}">
+  <dimension ref="A1:H105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B6" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B15" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B16" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B69" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B75" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B76" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B77" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B78" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B79" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B80" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B81" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B82" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B83" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B84" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B85" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B86" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B87" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B88" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B89" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B90" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B91" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B92" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B93" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B94" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B95" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B96" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B97" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B98" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B99" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B100" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B101" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B102" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B103" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B104" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B105" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated FIN_grids model - 2025-08-28 17:16
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_FIN_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4E33E2-0C74-4C8F-811C-4B569C58E33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD301ECF-3635-4114-A750-3433D67AC359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1150,7 +1150,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E2985C0-67F7-1572-8736-4A1C56069935}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9E186D-D8DC-58C7-83D3-B53ED1D0330B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1932,7 +1932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8FACE2-CC4B-4946-A187-073C83DEBD62}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742BC20A-774E-4248-82B6-A8C5391D8728}">
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>